<commit_message>
save Excel drama rating data
Save excel file : terrestrial and cable tv rating data (Nielsen) from
MySQL
Using pandas DataFrame

Formatting
id rate1 rate2 \n  <- weekly data
</commit_message>
<xml_diff>
--- a/cable_text.xlsx
+++ b/cable_text.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\develop\git_space\predictDramaRating\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="시청률흥행지표-케이블" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="predictSheet" sheetId="7" r:id="rId7"/>
     <sheet name="beforeAfter" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -792,7 +797,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -805,6 +810,2048 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictSheet!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>comment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>predictSheet!$D$2:$D$197</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="196"/>
+                <c:pt idx="0">
+                  <c:v>1.907</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0554999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.643</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6045</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3725000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4495000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8185000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0934999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0549999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.922000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.5625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.297000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.638500000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.298</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.983000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17.361499999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17.798500000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5075000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4984999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9044999999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.6345000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.427</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9184999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.548</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.9604999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.4205000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.4529999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.9325000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.7349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.8014999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.0564999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.2225000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.3599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.238</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2.5985</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.5594999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.0335000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.5700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.3049999999999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.504</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.7869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.6905000000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.4359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.0305</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.2389999999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.1034999999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.492</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.7789999999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.6370000000000005</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.9540000000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.5350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.5655000000000001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.4550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.7125000000000004</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.0145</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.0765000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.7945000000000002</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.4775</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.6239999999999997</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.669</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.468</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.3290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.6829999999999998</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5285000000000002</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.532</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.7410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.6245000000000003</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.5495000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.6040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.8940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.7235000000000014</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.93</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8.3825000000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.0274999999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9.0094999999999992</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.048</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.1814999999999998</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4794999999999998</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.3390000000000004</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.6180000000000003</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.7349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.4785000000000004</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.4039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.3325</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.3540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.4904999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.9824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.6799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.5155000000000003</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.7649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.952</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.0760000000000001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.8654999999999999</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.4314999999999998</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.9674999999999998</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.1029999999999998</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.1604999999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.6819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.8174999999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.9115</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.0819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2.8530000000000002</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.2404999999999999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2.7650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2.456</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2.859</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>7.9525000000000006</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>7.4329999999999998</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8.6120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7.7934999999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>9.8254999999999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>9.629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>10.3935</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>12.544</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.6870000000000003</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>6.3804999999999996</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>6.3900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6.8235000000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>5.7210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>6.4870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>6.6880000000000006</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>13.06</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>13.9955</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>15.282</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>12.464</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>13.06</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>13.9955</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>15.282</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>16.331499999999998</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>18.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.591</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1.6015000000000001</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2.3940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.9655</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.542</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.6395</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.899</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>5.6135000000000002</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>5.7195</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>6.0250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>6.5679999999999996</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>6.8680000000000003</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3.4785000000000004</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.5750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3.6310000000000002</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.8490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.7330000000000005</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>5.3945000000000007</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2.4609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2.0445000000000002</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.9060000000000001</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.8944999999999999</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2.0470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1.8319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.5805</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1.5834999999999999</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1.4495</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.3634999999999999</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1.3774999999999999</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.7885</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.6495000000000002</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1.8039999999999998</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2.1629999999999998</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2.089</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2.2210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2.1970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1.6415</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1.7635000000000001</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2.0419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1.5085000000000002</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1.802</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1.3774999999999999</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1.4039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>3.625</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>3.6539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>3.4939999999999998</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>3.3414999999999999</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>3.6905000000000001</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>4.5590000000000002</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>4.9655000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>predictSheet!$M$2:$M$197</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="196"/>
+                <c:pt idx="0">
+                  <c:v>957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>517</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1082</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1248</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5568</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6799</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6067</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8407</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9052</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8892</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12762</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1428</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1084</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1081</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1465</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1541</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1439</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1283</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1097</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1371</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>962</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1221</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>917</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>741</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1483</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>614</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>888</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2109</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2912</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3247</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8147</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4726</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4576</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2849</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3793</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1534</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>624</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1164</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>923</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1064</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>635</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>698</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>974</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>933</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1608</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>858</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1021</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1474</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2246</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2947</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2529</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2915</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3210</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>4248</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>4257</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2792</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>4934</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4609</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>5346</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>7154</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>7552</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>6314</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4945</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2870</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>593</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>594</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1387</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1666</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>12762</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>548.5</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>957</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1773728960"/>
+        <c:axId val="1773728416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1773728960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1773728416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1773728416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1773728960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1062,7 +3109,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -23679,8 +25726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="M198" sqref="M198"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" activeCellId="1" sqref="D1:D1048576 M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -31817,6 +33864,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31825,7 +33873,7 @@
   <dimension ref="A1:F193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>